<commit_message>
Subo ETL con datos actualizados
</commit_message>
<xml_diff>
--- a/resultado.xlsx
+++ b/resultado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -46,6 +46,36 @@
     <t>Pedro Salazar</t>
   </si>
   <si>
+    <t>María López</t>
+  </si>
+  <si>
+    <t>Jorge Medina</t>
+  </si>
+  <si>
+    <t>Rosa Castillo</t>
+  </si>
+  <si>
+    <t>Luis Fernández</t>
+  </si>
+  <si>
+    <t>Patricia Ríos</t>
+  </si>
+  <si>
+    <t>Miguel Quispe</t>
+  </si>
+  <si>
+    <t>Sandra Núñez</t>
+  </si>
+  <si>
+    <t>Renzo Valdivia</t>
+  </si>
+  <si>
+    <t>Carmen Soto</t>
+  </si>
+  <si>
+    <t>Diego Paredes</t>
+  </si>
+  <si>
     <t>Lima</t>
   </si>
   <si>
@@ -59,6 +89,33 @@
   </si>
   <si>
     <t>Piura</t>
+  </si>
+  <si>
+    <t>Chiclayo</t>
+  </si>
+  <si>
+    <t>Iquitos</t>
+  </si>
+  <si>
+    <t>Huaraz</t>
+  </si>
+  <si>
+    <t>Tacna</t>
+  </si>
+  <si>
+    <t>Puno</t>
+  </si>
+  <si>
+    <t>Ayacucho</t>
+  </si>
+  <si>
+    <t>Huancayo</t>
+  </si>
+  <si>
+    <t>Moquegua</t>
+  </si>
+  <si>
+    <t>Tumbes</t>
   </si>
 </sst>
 </file>
@@ -416,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,7 +507,7 @@
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>120</v>
@@ -467,7 +524,7 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>200</v>
@@ -484,7 +541,7 @@
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>150</v>
@@ -501,7 +558,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E5">
         <v>180</v>
@@ -518,10 +575,180 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subo proyecto ETL con limpieza de datos
</commit_message>
<xml_diff>
--- a/resultado.xlsx
+++ b/resultado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -34,88 +34,37 @@
     <t>Juan Perez</t>
   </si>
   <si>
-    <t>Ana Torres</t>
-  </si>
-  <si>
     <t>Carlos Ruiz</t>
   </si>
   <si>
     <t>Lucia Gomez</t>
   </si>
   <si>
-    <t>Pedro Salazar</t>
-  </si>
-  <si>
-    <t>María López</t>
-  </si>
-  <si>
     <t>Jorge Medina</t>
   </si>
   <si>
-    <t>Rosa Castillo</t>
-  </si>
-  <si>
-    <t>Luis Fernández</t>
-  </si>
-  <si>
-    <t>Patricia Ríos</t>
-  </si>
-  <si>
-    <t>Miguel Quispe</t>
-  </si>
-  <si>
-    <t>Sandra Núñez</t>
-  </si>
-  <si>
-    <t>Renzo Valdivia</t>
-  </si>
-  <si>
-    <t>Carmen Soto</t>
-  </si>
-  <si>
-    <t>Diego Paredes</t>
+    <t>Luis Fernandez</t>
+  </si>
+  <si>
+    <t>SIN NOMBRE</t>
   </si>
   <si>
     <t>Lima</t>
   </si>
   <si>
-    <t>Arequipa</t>
-  </si>
-  <si>
     <t>Trujillo</t>
   </si>
   <si>
-    <t>Cusco</t>
-  </si>
-  <si>
-    <t>Piura</t>
-  </si>
-  <si>
-    <t>Chiclayo</t>
+    <t>SIN CIUDAD</t>
   </si>
   <si>
     <t>Iquitos</t>
   </si>
   <si>
-    <t>Huaraz</t>
-  </si>
-  <si>
     <t>Tacna</t>
   </si>
   <si>
     <t>Puno</t>
-  </si>
-  <si>
-    <t>Ayacucho</t>
-  </si>
-  <si>
-    <t>Huancayo</t>
-  </si>
-  <si>
-    <t>Moquegua</t>
-  </si>
-  <si>
-    <t>Tumbes</t>
   </si>
 </sst>
 </file>
@@ -473,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,7 +456,7 @@
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>120</v>
@@ -515,240 +464,87 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>150</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E5">
-        <v>180</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E6">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E7">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11">
         <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16">
-        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>